<commit_message>
BRB session 0 data collection
</commit_message>
<xml_diff>
--- a/data/DND Dice Rolls.xlsx
+++ b/data/DND Dice Rolls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\DND_Dice_Rolls\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0F72A7-3DE6-4276-A023-3046DF0120B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DE4CE8-978C-4421-BC89-2B0A17347F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="2808" windowWidth="12960" windowHeight="7824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,6 +102,7 @@
 SR - Sunny River
 Campaign - campaign acronym
 FWM - Fae Wilds Merind
+BRB - Blue Ribbon Bakeoff
 Session - session number</t>
         </r>
       </text>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +157,18 @@
   <si>
     <t>ID_Number</t>
   </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>DB-MB-BRB-0</t>
+  </si>
+  <si>
+    <t>d12</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -182,6 +195,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -205,11 +225,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +461,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1098,12 +1127,24 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="A17" s="4">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="6">
+        <v>45585</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1127,12 +1168,24 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="4">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="6">
+        <v>45585</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1156,12 +1209,24 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="6">
+        <v>45585</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1185,12 +1250,24 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="6">
+        <v>45585</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1214,12 +1291,24 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6">
+        <v>45585</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1243,12 +1332,24 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="A22" s="4">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="6">
+        <v>45585</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1272,12 +1373,24 @@
       <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="6">
+        <v>45585</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1301,12 +1414,24 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="6">
+        <v>45585</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1330,12 +1455,24 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="A25" s="4">
+        <v>6</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="6">
+        <v>45585</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1359,12 +1496,24 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="6">
+        <v>45585</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1388,12 +1537,24 @@
       <c r="AA26" s="2"/>
     </row>
     <row r="27" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="6">
+        <v>45585</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1417,12 +1578,24 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="A28" s="4">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="6">
+        <v>45585</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1446,12 +1619,24 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="A29" s="4">
+        <v>5</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="6">
+        <v>45585</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1475,12 +1660,24 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="A30" s="4">
+        <v>5</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="6">
+        <v>45585</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1504,12 +1701,24 @@
       <c r="AA30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="6">
+        <v>45585</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -1533,12 +1742,24 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="A32" s="4">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="6">
+        <v>45585</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1562,12 +1783,24 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="A33" s="4">
+        <v>6</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="6">
+        <v>45585</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1591,12 +1824,24 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="A34" s="4">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="6">
+        <v>45585</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1620,12 +1865,24 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="6">
+        <v>45585</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1649,12 +1906,24 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="A36" s="4">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="6">
+        <v>45585</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -1678,12 +1947,24 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="A37" s="4">
+        <v>1</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="6">
+        <v>45585</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1707,12 +1988,24 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="A38" s="4">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="6">
+        <v>45585</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -1736,12 +2029,24 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="4">
+        <v>4</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="6">
+        <v>45585</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -1765,12 +2070,24 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="A40" s="4">
+        <v>6</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="6">
+        <v>45585</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -1794,12 +2111,24 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="A41" s="4">
+        <v>5</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="6">
+        <v>45585</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -1823,12 +2152,24 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="A42" s="4">
+        <v>3</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="6">
+        <v>45585</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -1852,12 +2193,24 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="A43" s="4">
+        <v>3</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="6">
+        <v>45585</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -1881,12 +2234,24 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="A44" s="4">
+        <v>5</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="6">
+        <v>45585</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -1910,12 +2275,24 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="A45" s="4">
+        <v>5</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="6">
+        <v>45585</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -1939,12 +2316,24 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="A46" s="4">
+        <v>4</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="6">
+        <v>45585</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -1968,12 +2357,24 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="A47" s="4">
+        <v>4</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="6">
+        <v>45585</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -1997,12 +2398,24 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="A48" s="4">
+        <v>4</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="6">
+        <v>45585</v>
+      </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -2026,12 +2439,24 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="A49" s="4">
+        <v>6</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="6">
+        <v>45585</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -2055,12 +2480,24 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="A50" s="4">
+        <v>2</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="6">
+        <v>45585</v>
+      </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -2084,12 +2521,24 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="A51" s="4">
+        <v>4</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="6">
+        <v>45585</v>
+      </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -2113,12 +2562,24 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="A52" s="4">
+        <v>5</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="6">
+        <v>45585</v>
+      </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -2142,12 +2603,24 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="A53" s="4">
+        <v>2</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="6">
+        <v>45585</v>
+      </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -2171,12 +2644,24 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="A54" s="4">
+        <v>1</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="6">
+        <v>45585</v>
+      </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -2200,12 +2685,24 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="A55" s="4">
+        <v>2</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="6">
+        <v>45585</v>
+      </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -2229,12 +2726,24 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="A56" s="4">
+        <v>5</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="6">
+        <v>45585</v>
+      </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -2258,12 +2767,24 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="A57" s="4">
+        <v>2</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="6">
+        <v>45585</v>
+      </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -2287,12 +2808,24 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="A58" s="4">
+        <v>2</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="6">
+        <v>45585</v>
+      </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -2316,12 +2849,24 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="A59" s="4">
+        <v>4</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="6">
+        <v>45585</v>
+      </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2345,12 +2890,24 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="A60" s="4">
+        <v>1</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="6">
+        <v>45585</v>
+      </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -2374,12 +2931,24 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="A61" s="4">
+        <v>5</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="6">
+        <v>45585</v>
+      </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -2403,12 +2972,24 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="A62" s="4">
+        <v>3</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="6">
+        <v>45585</v>
+      </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -2432,12 +3013,24 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="A63" s="4">
+        <v>2</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="6">
+        <v>45585</v>
+      </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -2461,12 +3054,24 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
+      <c r="A64" s="4">
+        <v>2</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="6">
+        <v>45585</v>
+      </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2490,12 +3095,24 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+      <c r="A65" s="4">
+        <v>5</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="6">
+        <v>45585</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -2519,12 +3136,24 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
+      <c r="A66" s="4">
+        <v>7</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="6">
+        <v>45585</v>
+      </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -2548,12 +3177,24 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
+      <c r="A67" s="4">
+        <v>6</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="6">
+        <v>45585</v>
+      </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2577,12 +3218,24 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+      <c r="A68" s="4">
+        <v>6</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="6">
+        <v>45585</v>
+      </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -29635,6 +30288,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started analysis for campaign BRB, and decided to use bar plots over dot plots
</commit_message>
<xml_diff>
--- a/data/DND Dice Rolls.xlsx
+++ b/data/DND Dice Rolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\DND_Dice_Rolls\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DE4CE8-978C-4421-BC89-2B0A17347F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E89383-FE7E-45D0-9E34-C6A4A37CDF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>d12</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -460,8 +463,8 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3177,8 +3180,8 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A67" s="4">
-        <v>6</v>
+      <c r="A67" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
fae wilds merind campaign die rolls data sheet and graph
</commit_message>
<xml_diff>
--- a/data/DND Dice Rolls.xlsx
+++ b/data/DND Dice Rolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\DND_Dice_Rolls\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E89383-FE7E-45D0-9E34-C6A4A37CDF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEEB48D-2A22-487C-84F6-142F4FCBDF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
             <scheme val="minor"/>
           </rPr>
           <t>What type of die was rolled 
-Options: d4, d6, d8, d10, d12, d20</t>
+Options: d4, d6, d8, d10, d%%, d12, d20</t>
         </r>
       </text>
     </comment>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -170,15 +170,19 @@
     <t>d12</t>
   </si>
   <si>
-    <t>s</t>
+    <t>d%%</t>
+  </si>
+  <si>
+    <t>d10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -239,7 +243,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -463,8 +467,8 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3180,8 +3184,8 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A67" s="4" t="s">
-        <v>14</v>
+      <c r="A67" s="4">
+        <v>12</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>1</v>
@@ -3262,12 +3266,24 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
+      <c r="A69" s="2">
+        <v>30</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="6">
+        <v>45585</v>
+      </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -3291,12 +3307,24 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15" x14ac:dyDescent="0.5">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="A70" s="2">
+        <v>9</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="6">
+        <v>45585</v>
+      </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>

</xml_diff>